<commit_message>
Back up of everything - needs curated later
</commit_message>
<xml_diff>
--- a/input/Polysaccharide degrading pathways.xlsx
+++ b/input/Polysaccharide degrading pathways.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idunmariaburgos/Documents/Work/Project/Ruminiclostridium cellulolyticum part 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idunmariaburgos/Ruminiclostridium_cellulolyticum_model/Ruminiclostridium-cellullolyticum-model-final/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682A96FD-C3E7-4347-A330-BBE1C34249CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A975FD1-CF72-2C4E-BCFF-3143A53215D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" firstSheet="2" activeTab="8" xr2:uid="{70959C0D-F7B0-5340-91FC-A6DCF411B3C0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="1" activeTab="7" xr2:uid="{70959C0D-F7B0-5340-91FC-A6DCF411B3C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Tamarind xyloglucan" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="457">
   <si>
     <t>Main substrate</t>
   </si>
@@ -729,9 +729,6 @@
     <t>{"M_cell3_c": -1,"M_pi_c": -1, "M_cellb_c": 1, "M_g1p_c":1}</t>
   </si>
   <si>
-    <t>C11H20O10</t>
-  </si>
-  <si>
     <t>Xylose</t>
   </si>
   <si>
@@ -756,9 +753,6 @@
     <t>Ccel_2456 and Ccel_2457 and Ccel_2458</t>
   </si>
   <si>
-    <t>C11H20O11</t>
-  </si>
-  <si>
     <t xml:space="preserve">Only included the CuaABC elements. CuaA is a solute binding protein that binds to all cellodextrins. CuaD only binds to cellobiose and has a higher affinity for this sugar. CuaD is essential for growth on cellobiose and cellulose. </t>
   </si>
   <si>
@@ -1353,54 +1347,6 @@
     <t>R_GQQGabc</t>
   </si>
   <si>
-    <t>{"M_cellb_e":-1, "M_atp_c":-2, "M_h2o_c":-1, "M_cellb_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
-  </si>
-  <si>
-    <t>{"M_cell3_e":-1, "M_atp_c":-2, "M_h2o_c":-1, "M_cell3_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
-  </si>
-  <si>
-    <t>{"M_cell4_e":-1, "M_atp_c":-2, "M_h2o_c":-1, "M_cell4_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
-  </si>
-  <si>
-    <t>{"M_cell5_e":-1, "M_atp_c":-2, "M_h2o_c":-1, "M_cell5_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
-  </si>
-  <si>
-    <t>{"M_AX_e":-1, "M_atp_c":-2, "M_h2o_c":-1, "M_AX_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
-  </si>
-  <si>
-    <t>{"M_AXX_e":-1, "M_atp_c":-2, "M_h2o_c":-1, "M_AXX_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
-  </si>
-  <si>
-    <t>{"M_A23XX_e":-1, "M_atp_c":-2, "M_h2o_c":-1, "M_A23XX_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
-  </si>
-  <si>
-    <t>{"M_XA23XX_e":-1, "M_atp_c":-2, "M_h2o_c":-1, "M_XA23XX_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
-  </si>
-  <si>
-    <t>{"M_XAXX_e":-1, "M_atp_c":-2, "M_h2o_c":-1, "M_XAXX_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
-  </si>
-  <si>
-    <t>{"M_QLQG_e":-1, "M_atp_c":-2, "M_h2o_c":-1, "M_QLQG_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
-  </si>
-  <si>
-    <t>{"M_QQLG_e":-1, "M_atp_c":-2, "M_h2o_c":-1, "M_QQLG_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
-  </si>
-  <si>
-    <t>{"M_QLLG_e":-1, "M_atp_c":-2, "M_h2o_c":-1, "M_QLLG_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
-  </si>
-  <si>
-    <t>{"M_QQQG_e":-1, "M_atp_c":-2, "M_h2o_c":-1, "M_QQQG_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
-  </si>
-  <si>
-    <t>{"M_GQQG_e":-1, "M_atp_c":-2, "M_h2o_c":-1, "M_GQQG_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
-  </si>
-  <si>
-    <t>XYLqg</t>
-  </si>
-  <si>
-    <t>GLUgqg</t>
-  </si>
-  <si>
     <t>M_xyl3_e</t>
   </si>
   <si>
@@ -1429,6 +1375,48 @@
   </si>
   <si>
     <t>M_cellb_e</t>
+  </si>
+  <si>
+    <t>{"M_QLLG_e":-1, "M_atp_c":-2, "M_h2o_c":-2, "M_QLLG_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
+  </si>
+  <si>
+    <t>{"M_QLQG_e":-1, "M_atp_c":-2, "M_h2o_c":-2, "M_QLQG_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
+  </si>
+  <si>
+    <t>{"M_QQLG_e":-1, "M_atp_c":-2, "M_h2o_c":-2, "M_QQLG_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
+  </si>
+  <si>
+    <t>{"M_QQQG_e":-1, "M_atp_c":-2, "M_h2o_c":-2, "M_QQQG_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
+  </si>
+  <si>
+    <t>{"M_GQQG_e":-1, "M_atp_c":-2, "M_h2o_c":-2, "M_GQQG_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
+  </si>
+  <si>
+    <t>{"M_cellb_e":-1, "M_atp_c":-2, "M_h2o_c":-2, "M_cellb_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
+  </si>
+  <si>
+    <t>{"M_cell3_e":-1, "M_atp_c":-2, "M_h2o_c":-2, "M_cell3_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
+  </si>
+  <si>
+    <t>{"M_cell4_e":-1, "M_atp_c":-2, "M_h2o_c":-2, "M_cell4_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
+  </si>
+  <si>
+    <t>{"M_cell5_e":-1, "M_atp_c":-2, "M_h2o_c":-2, "M_cell5_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
+  </si>
+  <si>
+    <t>{"M_AX_e":-1, "M_atp_c":-2, "M_h2o_c":-2, "M_AX_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
+  </si>
+  <si>
+    <t>{"M_AXX_e":-1, "M_atp_c":-2, "M_h2o_c":-2, "M_AXX_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
+  </si>
+  <si>
+    <t>{"M_A23XX_e":-1, "M_atp_c":-2, "M_h2o_c":-2, "M_A23XX_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
+  </si>
+  <si>
+    <t>{"M_XA23XX_e":-1, "M_atp_c":-2, "M_h2o_c":-2, "M_XA23XX_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
+  </si>
+  <si>
+    <t>{"M_XAXX_e":-1, "M_atp_c":-2, "M_h2o_c":-2, "M_XAXX_c":1, "M_adp_c":2,"M_h_c":2, "M_pi_c":2}</t>
   </si>
 </sst>
 </file>
@@ -1770,9 +1758,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1810,7 +1798,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1916,7 +1904,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2058,7 +2046,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2134,7 +2122,7 @@
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="H3" t="s">
         <v>17</v>
@@ -2172,7 +2160,7 @@
         <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="H4" t="s">
         <v>17</v>
@@ -2187,7 +2175,7 @@
         <v>173</v>
       </c>
       <c r="Q4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="R4" t="s">
         <v>9</v>
@@ -2213,7 +2201,7 @@
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="H5" t="s">
         <v>17</v>
@@ -2254,7 +2242,7 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H6" t="s">
         <v>17</v>
@@ -2292,7 +2280,7 @@
         <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="H7" t="s">
         <v>17</v>
@@ -2324,7 +2312,7 @@
         <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="H8" t="s">
         <v>17</v>
@@ -2356,7 +2344,7 @@
         <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="H9" t="s">
         <v>17</v>
@@ -2388,7 +2376,7 @@
         <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H10" t="s">
         <v>17</v>
@@ -2452,7 +2440,7 @@
         <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="H12" t="s">
         <v>17</v>
@@ -2487,7 +2475,7 @@
         <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="H13" t="s">
         <v>17</v>
@@ -2522,7 +2510,7 @@
         <v>14</v>
       </c>
       <c r="G14" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="H14" t="s">
         <v>17</v>
@@ -2557,7 +2545,7 @@
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H15" t="s">
         <v>17</v>
@@ -2624,7 +2612,7 @@
         <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="H17" t="s">
         <v>17</v>
@@ -2659,7 +2647,7 @@
         <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H18" t="s">
         <v>17</v>
@@ -2694,7 +2682,7 @@
         <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="H19" t="s">
         <v>17</v>
@@ -2729,7 +2717,7 @@
         <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H20" t="s">
         <v>17</v>
@@ -2798,7 +2786,7 @@
         <v>35</v>
       </c>
       <c r="G24" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="H24" t="s">
         <v>32</v>
@@ -2867,10 +2855,10 @@
         <v>50</v>
       </c>
       <c r="F29" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G29" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="H29" t="s">
         <v>59</v>
@@ -2899,10 +2887,10 @@
         <v>50</v>
       </c>
       <c r="F30" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G30" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="H30" t="s">
         <v>59</v>
@@ -2931,10 +2919,10 @@
         <v>50</v>
       </c>
       <c r="F31" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G31" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="H31" t="s">
         <v>59</v>
@@ -2963,10 +2951,10 @@
         <v>49</v>
       </c>
       <c r="F32" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="G32" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="H32" t="s">
         <v>59</v>
@@ -2995,10 +2983,10 @@
         <v>51</v>
       </c>
       <c r="F33" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="G33" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="H33" t="s">
         <v>59</v>
@@ -3027,10 +3015,10 @@
         <v>49</v>
       </c>
       <c r="F34" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G34" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="H34" t="s">
         <v>59</v>
@@ -3059,10 +3047,10 @@
         <v>51</v>
       </c>
       <c r="F35" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="G35" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="H35" t="s">
         <v>59</v>
@@ -3091,7 +3079,7 @@
         <v>49</v>
       </c>
       <c r="F36" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="G36" t="s">
         <v>63</v>
@@ -3139,36 +3127,36 @@
         <v>198</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>53</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>455</v>
+        <v>437</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q1" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>231</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>456</v>
+        <v>438</v>
       </c>
       <c r="B2" t="s">
-        <v>453</v>
+        <v>435</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>56</v>
@@ -3181,13 +3169,13 @@
         <v>0</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>455</v>
+        <v>437</v>
       </c>
       <c r="L2" t="s">
-        <v>453</v>
+        <v>435</v>
       </c>
       <c r="M2">
         <v>8</v>
@@ -3214,10 +3202,10 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>457</v>
+        <v>439</v>
       </c>
       <c r="B3" t="s">
-        <v>454</v>
+        <v>436</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>56</v>
@@ -3230,7 +3218,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H3">
         <v>5</v>
@@ -3239,7 +3227,7 @@
         <v>6</v>
       </c>
       <c r="L3" t="s">
-        <v>454</v>
+        <v>436</v>
       </c>
       <c r="M3">
         <v>4</v>
@@ -3266,10 +3254,10 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>458</v>
+        <v>440</v>
       </c>
       <c r="B4" t="s">
-        <v>451</v>
+        <v>433</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>56</v>
@@ -3282,7 +3270,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H4">
         <v>10</v>
@@ -3291,7 +3279,7 @@
         <v>10</v>
       </c>
       <c r="L4" t="s">
-        <v>451</v>
+        <v>433</v>
       </c>
       <c r="M4">
         <v>3</v>
@@ -3318,10 +3306,10 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>459</v>
+        <v>441</v>
       </c>
       <c r="B5" t="s">
-        <v>452</v>
+        <v>434</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>56</v>
@@ -3334,7 +3322,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H5">
         <v>5</v>
@@ -3343,7 +3331,7 @@
         <v>7</v>
       </c>
       <c r="L5" t="s">
-        <v>452</v>
+        <v>434</v>
       </c>
       <c r="M5">
         <v>2</v>
@@ -3378,8 +3366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6750B204-21B1-A54D-9F94-97EF63BB6BC9}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3627,7 +3615,7 @@
   <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3671,7 +3659,7 @@
         <v>2</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>165</v>
@@ -3679,13 +3667,13 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
         <v>444</v>
@@ -3711,13 +3699,13 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B3" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D3" t="s">
         <v>445</v>
@@ -3743,16 +3731,16 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B4" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D4" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -3775,16 +3763,16 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B5" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -3807,16 +3795,16 @@
     </row>
     <row r="6" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -3839,16 +3827,16 @@
     </row>
     <row r="7" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E7" s="4">
         <v>0</v>
@@ -3869,7 +3857,7 @@
         <v>59</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>216</v>
@@ -3877,16 +3865,16 @@
     </row>
     <row r="8" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E8" s="4">
         <v>0</v>
@@ -3907,7 +3895,7 @@
         <v>59</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="L8" s="4" t="s">
         <v>216</v>
@@ -3915,16 +3903,16 @@
     </row>
     <row r="9" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E9" s="4">
         <v>0</v>
@@ -3945,7 +3933,7 @@
         <v>59</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>216</v>
@@ -3953,16 +3941,16 @@
     </row>
     <row r="10" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E10" s="4">
         <v>0</v>
@@ -3983,7 +3971,7 @@
         <v>59</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>217</v>
@@ -3991,16 +3979,16 @@
     </row>
     <row r="11" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E11" s="4">
         <v>0</v>
@@ -4021,7 +4009,7 @@
         <v>59</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>220</v>
@@ -4029,16 +4017,16 @@
     </row>
     <row r="12" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E12" s="4">
         <v>0</v>
@@ -4059,7 +4047,7 @@
         <v>59</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>217</v>
@@ -4067,16 +4055,16 @@
     </row>
     <row r="13" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E13" s="4">
         <v>0</v>
@@ -4097,7 +4085,7 @@
         <v>59</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>220</v>
@@ -4105,16 +4093,16 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E14" s="4">
         <v>0</v>
@@ -4135,7 +4123,7 @@
         <v>59</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>217</v>
@@ -4180,9 +4168,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
-      <c r="B19" s="4" t="s">
-        <v>449</v>
-      </c>
+      <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="F19" s="4"/>
@@ -4190,11 +4176,6 @@
       <c r="H19" s="4"/>
       <c r="J19" s="4"/>
       <c r="L19" s="4"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>450</v>
-      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
@@ -4214,8 +4195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{416C2792-2A02-F945-A022-0626127C656A}">
   <dimension ref="A1:V14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4237,7 +4218,7 @@
         <v>198</v>
       </c>
       <c r="H1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M1" t="s">
         <v>53</v>
@@ -4246,22 +4227,22 @@
         <v>207</v>
       </c>
       <c r="O1" t="s">
+        <v>227</v>
+      </c>
+      <c r="P1" t="s">
         <v>228</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
+        <v>233</v>
+      </c>
+      <c r="S1" t="s">
         <v>229</v>
       </c>
-      <c r="Q1" t="s">
-        <v>234</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>230</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>231</v>
-      </c>
-      <c r="U1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
@@ -4269,13 +4250,13 @@
         <v>208</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C2" t="s">
         <v>56</v>
       </c>
       <c r="D2" t="str">
-        <f>"C"&amp;S2&amp;"H"&amp;T2&amp;"O"&amp;U2</f>
+        <f t="shared" ref="D2:D14" si="0">"C"&amp;S2&amp;"H"&amp;T2&amp;"O"&amp;U2</f>
         <v>C45H76O38</v>
       </c>
       <c r="E2">
@@ -4285,13 +4266,13 @@
         <v>207</v>
       </c>
       <c r="J2" t="s">
+        <v>227</v>
+      </c>
+      <c r="K2" t="s">
         <v>228</v>
       </c>
-      <c r="K2" t="s">
-        <v>229</v>
-      </c>
       <c r="M2" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="N2">
         <v>4</v>
@@ -4315,7 +4296,7 @@
         <v>76</v>
       </c>
       <c r="U2">
-        <f t="shared" ref="U2:U14" si="0">N2*$I$5+O2*$J$5+P2*$K$5-Q2</f>
+        <f t="shared" ref="U2:U14" si="1">N2*$I$5+O2*$J$5+P2*$K$5-Q2</f>
         <v>38</v>
       </c>
     </row>
@@ -4324,20 +4305,20 @@
         <v>209</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C3" t="s">
         <v>56</v>
       </c>
       <c r="D3" t="str">
-        <f>"C"&amp;S3&amp;"H"&amp;T3&amp;"O"&amp;U3</f>
+        <f t="shared" si="0"/>
         <v>C45H76O38</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I3">
         <v>6</v>
@@ -4349,7 +4330,7 @@
         <v>6</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="N3">
         <v>4</v>
@@ -4361,19 +4342,19 @@
         <v>1</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q12" si="1">SUM(N3:P3)-1</f>
+        <f t="shared" ref="Q3:Q12" si="2">SUM(N3:P3)-1</f>
         <v>7</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S14" si="2">N3*$I$3+O3*$J$3+P3*$K$3</f>
+        <f t="shared" ref="S3:S14" si="3">N3*$I$3+O3*$J$3+P3*$K$3</f>
         <v>45</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:T14" si="3">N3*$I$4+O3*$J$4+P3*$K$4-2*Q3</f>
+        <f t="shared" ref="T3:T14" si="4">N3*$I$4+O3*$J$4+P3*$K$4-2*Q3</f>
         <v>76</v>
       </c>
       <c r="U3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
     </row>
@@ -4382,20 +4363,20 @@
         <v>210</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C4" t="s">
         <v>56</v>
       </c>
       <c r="D4" t="str">
-        <f>"C"&amp;S4&amp;"H"&amp;T4&amp;"O"&amp;U4</f>
+        <f t="shared" si="0"/>
         <v>C51H86O43</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I4">
         <v>12</v>
@@ -4407,7 +4388,7 @@
         <v>12</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="N4">
         <v>4</v>
@@ -4419,19 +4400,19 @@
         <v>2</v>
       </c>
       <c r="Q4">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="4"/>
+        <v>86</v>
+      </c>
+      <c r="U4">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="S4">
-        <f t="shared" si="2"/>
-        <v>51</v>
-      </c>
-      <c r="T4">
-        <f t="shared" si="3"/>
-        <v>86</v>
-      </c>
-      <c r="U4">
-        <f t="shared" si="0"/>
         <v>43</v>
       </c>
     </row>
@@ -4440,20 +4421,20 @@
         <v>211</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C5" t="s">
         <v>56</v>
       </c>
       <c r="D5" t="str">
-        <f>"C"&amp;S5&amp;"H"&amp;T5&amp;"O"&amp;U5</f>
+        <f t="shared" si="0"/>
         <v>C39H66O33</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I5">
         <v>6</v>
@@ -4465,7 +4446,7 @@
         <v>6</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="N5">
         <v>4</v>
@@ -4477,19 +4458,19 @@
         <v>0</v>
       </c>
       <c r="Q5">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="4"/>
+        <v>66</v>
+      </c>
+      <c r="U5">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="S5">
-        <f t="shared" si="2"/>
-        <v>39</v>
-      </c>
-      <c r="T5">
-        <f t="shared" si="3"/>
-        <v>66</v>
-      </c>
-      <c r="U5">
-        <f t="shared" si="0"/>
         <v>33</v>
       </c>
     </row>
@@ -4498,20 +4479,20 @@
         <v>208</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C6" t="s">
         <v>58</v>
       </c>
       <c r="D6" t="str">
-        <f>"C"&amp;S6&amp;"H"&amp;T6&amp;"O"&amp;U6</f>
+        <f t="shared" si="0"/>
         <v>C45H76O38</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="N6">
         <v>4</v>
@@ -4523,19 +4504,19 @@
         <v>1</v>
       </c>
       <c r="Q6">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="4"/>
+        <v>76</v>
+      </c>
+      <c r="U6">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="S6">
-        <f t="shared" si="2"/>
-        <v>45</v>
-      </c>
-      <c r="T6">
-        <f t="shared" si="3"/>
-        <v>76</v>
-      </c>
-      <c r="U6">
-        <f t="shared" si="0"/>
         <v>38</v>
       </c>
     </row>
@@ -4544,20 +4525,20 @@
         <v>209</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C7" t="s">
         <v>58</v>
       </c>
       <c r="D7" t="str">
-        <f>"C"&amp;S7&amp;"H"&amp;T7&amp;"O"&amp;U7</f>
+        <f t="shared" si="0"/>
         <v>C45H76O38</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="N7">
         <v>4</v>
@@ -4569,19 +4550,19 @@
         <v>1</v>
       </c>
       <c r="Q7">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="4"/>
+        <v>76</v>
+      </c>
+      <c r="U7">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="S7">
-        <f t="shared" si="2"/>
-        <v>45</v>
-      </c>
-      <c r="T7">
-        <f t="shared" si="3"/>
-        <v>76</v>
-      </c>
-      <c r="U7">
-        <f t="shared" si="0"/>
         <v>38</v>
       </c>
     </row>
@@ -4590,20 +4571,20 @@
         <v>210</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C8" t="s">
         <v>58</v>
       </c>
       <c r="D8" t="str">
-        <f>"C"&amp;S8&amp;"H"&amp;T8&amp;"O"&amp;U8</f>
+        <f t="shared" si="0"/>
         <v>C51H86O43</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="N8">
         <v>4</v>
@@ -4615,19 +4596,19 @@
         <v>2</v>
       </c>
       <c r="Q8">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="4"/>
+        <v>86</v>
+      </c>
+      <c r="U8">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="S8">
-        <f t="shared" si="2"/>
-        <v>51</v>
-      </c>
-      <c r="T8">
-        <f t="shared" si="3"/>
-        <v>86</v>
-      </c>
-      <c r="U8">
-        <f t="shared" si="0"/>
         <v>43</v>
       </c>
     </row>
@@ -4636,20 +4617,20 @@
         <v>211</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C9" t="s">
         <v>58</v>
       </c>
       <c r="D9" t="str">
-        <f>"C"&amp;S9&amp;"H"&amp;T9&amp;"O"&amp;U9</f>
+        <f t="shared" si="0"/>
         <v>C39H66O33</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="N9" s="4">
         <v>4</v>
@@ -4661,20 +4642,20 @@
         <v>0</v>
       </c>
       <c r="Q9" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="R9" s="4"/>
       <c r="S9" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="T9" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>66</v>
       </c>
       <c r="U9" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
     </row>
@@ -4683,13 +4664,13 @@
         <v>212</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C10" t="s">
         <v>58</v>
       </c>
       <c r="D10" t="str">
-        <f>"C"&amp;S10&amp;"H"&amp;T10&amp;"O"&amp;U10</f>
+        <f t="shared" si="0"/>
         <v>C34H58O29</v>
       </c>
       <c r="E10">
@@ -4701,7 +4682,7 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="N10">
         <v>4</v>
@@ -4713,19 +4694,19 @@
         <v>0</v>
       </c>
       <c r="Q10">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="4"/>
+        <v>58</v>
+      </c>
+      <c r="U10">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="S10">
-        <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="T10">
-        <f t="shared" si="3"/>
-        <v>58</v>
-      </c>
-      <c r="U10">
-        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="V10" s="4"/>
@@ -4735,20 +4716,20 @@
         <v>213</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C11" t="s">
         <v>58</v>
       </c>
       <c r="D11" t="str">
-        <f>"C"&amp;S11&amp;"H"&amp;T11&amp;"O"&amp;U11</f>
+        <f t="shared" si="0"/>
         <v>C28H48O24</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="N11">
         <v>3</v>
@@ -4760,19 +4741,19 @@
         <v>0</v>
       </c>
       <c r="Q11">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="U11">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="S11">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="T11">
-        <f t="shared" si="3"/>
-        <v>48</v>
-      </c>
-      <c r="U11">
-        <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
@@ -4781,13 +4762,13 @@
         <v>214</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C12" t="s">
         <v>58</v>
       </c>
       <c r="D12" t="str">
-        <f>"C"&amp;S12&amp;"H"&amp;T12&amp;"O"&amp;U12</f>
+        <f t="shared" si="0"/>
         <v>C23H40O20</v>
       </c>
       <c r="E12">
@@ -4798,7 +4779,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="N12">
         <v>3</v>
@@ -4810,19 +4791,19 @@
         <v>0</v>
       </c>
       <c r="Q12">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="U12">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="S12">
-        <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="T12">
-        <f t="shared" si="3"/>
-        <v>40</v>
-      </c>
-      <c r="U12">
-        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -4831,19 +4812,20 @@
         <v>215</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C13" t="s">
         <v>58</v>
       </c>
-      <c r="D13" t="s">
-        <v>227</v>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>C17H30O15</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="N13">
         <v>2</v>
@@ -4867,7 +4849,7 @@
         <v>30</v>
       </c>
       <c r="U13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
@@ -4876,13 +4858,14 @@
         <v>212</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D14" t="s">
-        <v>236</v>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>C34H58O29</v>
       </c>
       <c r="E14" s="4">
         <v>0</v>
@@ -4893,7 +4876,7 @@
       <c r="K14"/>
       <c r="L14"/>
       <c r="M14" s="4" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="N14">
         <v>4</v>
@@ -4910,15 +4893,15 @@
       </c>
       <c r="R14"/>
       <c r="S14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
       <c r="T14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>58</v>
       </c>
       <c r="U14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="V14"/>
@@ -5589,7 +5572,7 @@
         <v>57</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K29" s="7" t="s">
         <v>184</v>
@@ -5600,7 +5583,7 @@
         <v>86</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>87</v>
@@ -5609,16 +5592,16 @@
         <v>54</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I30" s="8" t="s">
         <v>57</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K30" s="8" t="s">
         <v>184</v>
@@ -5738,7 +5721,7 @@
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -5771,7 +5754,7 @@
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="4" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -5804,7 +5787,7 @@
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -5823,7 +5806,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView zoomScale="111" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5872,13 +5855,13 @@
         <v>201</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>88</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>435</v>
+        <v>448</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -5904,13 +5887,13 @@
         <v>203</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>88</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>436</v>
+        <v>449</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -5939,13 +5922,13 @@
         <v>202</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>88</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>437</v>
+        <v>450</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -5971,13 +5954,13 @@
         <v>204</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>88</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>438</v>
+        <v>451</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -6000,13 +5983,13 @@
     </row>
     <row r="6" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>224</v>
@@ -6044,7 +6027,7 @@
         <v>205</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>97</v>
@@ -6079,7 +6062,7 @@
         <v>206</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>94</v>
@@ -6170,7 +6153,7 @@
         <v>198</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>53</v>
@@ -6179,16 +6162,16 @@
         <v>207</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q1" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>231</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -6223,15 +6206,15 @@
         <v>4</v>
       </c>
       <c r="Q2">
-        <f>M2*$H$3</f>
+        <f t="shared" ref="Q2:Q8" si="0">M2*$H$3</f>
         <v>30</v>
       </c>
       <c r="R2">
-        <f>M2*$H$4-2*N2</f>
+        <f t="shared" ref="R2:R8" si="1">M2*$H$4-2*N2</f>
         <v>52</v>
       </c>
       <c r="S2">
-        <f>M2*$H$5-N2</f>
+        <f t="shared" ref="S2:S8" si="2">M2*$H$5-N2</f>
         <v>26</v>
       </c>
     </row>
@@ -6246,14 +6229,14 @@
         <v>58</v>
       </c>
       <c r="D3" s="4" t="str">
-        <f t="shared" ref="D3:D7" si="0">"C"&amp;Q3&amp;"H"&amp;R3&amp;"O"&amp;S3</f>
+        <f t="shared" ref="D3:D7" si="3">"C"&amp;Q3&amp;"H"&amp;R3&amp;"O"&amp;S3</f>
         <v>C30H52O26</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -6265,19 +6248,19 @@
         <v>5</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N8" si="1">SUM(M3)-1</f>
+        <f t="shared" ref="N3:N8" si="4">SUM(M3)-1</f>
         <v>4</v>
       </c>
       <c r="Q3">
-        <f>M3*$H$3</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="R3">
-        <f>M3*$H$4-2*N3</f>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="S3">
-        <f>M3*$H$5-N3</f>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
     </row>
@@ -6292,14 +6275,14 @@
         <v>56</v>
       </c>
       <c r="D4" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>C24H42O21</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H4">
         <v>12</v>
@@ -6311,19 +6294,19 @@
         <v>4</v>
       </c>
       <c r="N4">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="R4">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="Q4">
-        <f>M4*$H$3</f>
-        <v>24</v>
-      </c>
-      <c r="R4">
-        <f>M4*$H$4-2*N4</f>
         <v>42</v>
       </c>
       <c r="S4">
-        <f>M4*$H$5-N4</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
     </row>
@@ -6338,14 +6321,14 @@
         <v>58</v>
       </c>
       <c r="D5" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>C24H42O21</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H5">
         <v>6</v>
@@ -6357,19 +6340,19 @@
         <v>4</v>
       </c>
       <c r="N5">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="R5">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="Q5">
-        <f>M5*$H$3</f>
-        <v>24</v>
-      </c>
-      <c r="R5">
-        <f>M5*$H$4-2*N5</f>
         <v>42</v>
       </c>
       <c r="S5">
-        <f>M5*$H$5-N5</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
     </row>
@@ -6397,19 +6380,19 @@
         <v>3</v>
       </c>
       <c r="N6">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="R6">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="Q6">
-        <f>M6*$H$3</f>
-        <v>18</v>
-      </c>
-      <c r="R6">
-        <f>M6*$H$4-2*N6</f>
         <v>32</v>
       </c>
       <c r="S6">
-        <f>M6*$H$5-N6</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
     </row>
@@ -6424,7 +6407,7 @@
         <v>58</v>
       </c>
       <c r="D7" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>C18H32O16</v>
       </c>
       <c r="E7">
@@ -6437,43 +6420,43 @@
         <v>3</v>
       </c>
       <c r="N7">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="R7">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="Q7">
-        <f>M7*$H$3</f>
-        <v>18</v>
-      </c>
-      <c r="R7">
-        <f>M7*$H$4-2*N7</f>
         <v>32</v>
       </c>
       <c r="S7">
-        <f>M7*$H$5-N7</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="L8" t="s">
-        <v>460</v>
+        <v>442</v>
       </c>
       <c r="M8">
         <v>2</v>
       </c>
       <c r="N8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="R8">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Q8">
-        <f>M8*$H$3</f>
-        <v>12</v>
-      </c>
-      <c r="R8">
-        <f>M8*$H$4-2*N8</f>
         <v>22</v>
       </c>
       <c r="S8">
-        <f>M8*$H$5-N8</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
     </row>
@@ -6544,7 +6527,7 @@
         <v>18</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>165</v>
@@ -6552,738 +6535,738 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C3" t="s">
         <v>242</v>
-      </c>
-      <c r="B3" t="s">
-        <v>243</v>
-      </c>
-      <c r="C3" t="s">
-        <v>244</v>
       </c>
       <c r="D3" t="s">
         <v>54</v>
       </c>
       <c r="E3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I3" t="s">
         <v>57</v>
       </c>
       <c r="J3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>240</v>
+      </c>
+      <c r="B4" t="s">
+        <v>241</v>
+      </c>
+      <c r="C4" t="s">
         <v>242</v>
-      </c>
-      <c r="B4" t="s">
-        <v>243</v>
-      </c>
-      <c r="C4" t="s">
-        <v>244</v>
       </c>
       <c r="D4" t="s">
         <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I4" t="s">
         <v>57</v>
       </c>
       <c r="J4" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="L4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C5" t="s">
         <v>242</v>
-      </c>
-      <c r="B5" t="s">
-        <v>243</v>
-      </c>
-      <c r="C5" t="s">
-        <v>244</v>
       </c>
       <c r="D5" t="s">
         <v>54</v>
       </c>
       <c r="E5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F5" t="s">
         <v>245</v>
       </c>
-      <c r="F5" t="s">
-        <v>247</v>
-      </c>
       <c r="G5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I5" t="s">
         <v>57</v>
       </c>
       <c r="J5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>240</v>
+      </c>
+      <c r="B6" t="s">
+        <v>241</v>
+      </c>
+      <c r="C6" t="s">
         <v>242</v>
-      </c>
-      <c r="B6" t="s">
-        <v>243</v>
-      </c>
-      <c r="C6" t="s">
-        <v>244</v>
       </c>
       <c r="D6" t="s">
         <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I6" t="s">
         <v>57</v>
       </c>
       <c r="J6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>240</v>
+      </c>
+      <c r="B7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C7" t="s">
         <v>242</v>
-      </c>
-      <c r="B7" t="s">
-        <v>243</v>
-      </c>
-      <c r="C7" t="s">
-        <v>244</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I7" t="s">
         <v>57</v>
       </c>
       <c r="J7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L7" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D8" t="s">
         <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G8" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="H8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I8" t="s">
         <v>58</v>
       </c>
       <c r="J8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="K8" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="L8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C9" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D9" t="s">
         <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G9" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="H9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I9" t="s">
         <v>58</v>
       </c>
       <c r="J9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="K9" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="L9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B10" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C10" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D10" t="s">
         <v>54</v>
       </c>
       <c r="E10" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F10" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I10" t="s">
         <v>58</v>
       </c>
       <c r="J10" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="K10" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="L10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D11" t="s">
         <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G11" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I11" t="s">
         <v>58</v>
       </c>
       <c r="J11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="K11" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="L11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C12" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D12" t="s">
         <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F12" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G12" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I12" t="s">
         <v>58</v>
       </c>
       <c r="J12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="K12" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="L12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B13" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C13" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D13" t="s">
         <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F13" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G13" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H13" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I13" t="s">
         <v>58</v>
       </c>
       <c r="J13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="K13" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="L13" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B14" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C14" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D14" t="s">
         <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F14" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G14" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="H14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I14" t="s">
         <v>58</v>
       </c>
       <c r="J14" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="K14" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="L14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B15" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C15" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D15" t="s">
         <v>54</v>
       </c>
       <c r="E15" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F15" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G15" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="H15" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I15" t="s">
         <v>58</v>
       </c>
       <c r="J15" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="K15" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="L15" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B16" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C16" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D16" t="s">
         <v>54</v>
       </c>
       <c r="E16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F16" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G16" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="H16" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I16" t="s">
         <v>58</v>
       </c>
       <c r="J16" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="K16" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="L16" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B17" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C17" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D17" t="s">
         <v>54</v>
       </c>
       <c r="E17" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F17" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G17" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="H17" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I17" t="s">
         <v>58</v>
       </c>
       <c r="J17" t="s">
+        <v>344</v>
+      </c>
+      <c r="K17" t="s">
         <v>346</v>
       </c>
-      <c r="K17" t="s">
-        <v>348</v>
-      </c>
       <c r="L17" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B18" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C18" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D18" t="s">
         <v>54</v>
       </c>
       <c r="E18" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G18" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="H18" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I18" t="s">
         <v>58</v>
       </c>
       <c r="J18" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="L18" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B19" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C19" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D19" t="s">
         <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G19" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="H19" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I19" t="s">
         <v>58</v>
       </c>
       <c r="J19" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="L19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B20" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C20" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D20" t="s">
         <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F20" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G20" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="H20" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I20" t="s">
         <v>58</v>
       </c>
       <c r="J20" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="L20" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B21" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D21" t="s">
         <v>54</v>
       </c>
       <c r="E21" t="s">
+        <v>260</v>
+      </c>
+      <c r="F21" t="s">
+        <v>246</v>
+      </c>
+      <c r="G21" t="s">
+        <v>354</v>
+      </c>
+      <c r="H21" t="s">
         <v>262</v>
-      </c>
-      <c r="F21" t="s">
-        <v>248</v>
-      </c>
-      <c r="G21" t="s">
-        <v>356</v>
-      </c>
-      <c r="H21" t="s">
-        <v>264</v>
       </c>
       <c r="I21" t="s">
         <v>58</v>
       </c>
       <c r="J21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="K21" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="L21" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B22" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D22" t="s">
         <v>54</v>
       </c>
       <c r="E22" t="s">
+        <v>260</v>
+      </c>
+      <c r="F22" t="s">
+        <v>263</v>
+      </c>
+      <c r="G22" t="s">
+        <v>355</v>
+      </c>
+      <c r="H22" t="s">
         <v>262</v>
-      </c>
-      <c r="F22" t="s">
-        <v>265</v>
-      </c>
-      <c r="G22" t="s">
-        <v>357</v>
-      </c>
-      <c r="H22" t="s">
-        <v>264</v>
       </c>
       <c r="I22" t="s">
         <v>58</v>
       </c>
       <c r="J22" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="K22" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="L22" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7299,8 +7282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FEF6FD-B447-CB42-96EE-A5346513752C}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7338,16 +7321,16 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>439</v>
+        <v>452</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -7359,21 +7342,21 @@
         <v>54</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>440</v>
+        <v>453</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -7385,21 +7368,21 @@
         <v>54</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>441</v>
+        <v>454</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -7411,21 +7394,21 @@
         <v>54</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>442</v>
+        <v>455</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -7437,21 +7420,21 @@
         <v>54</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>443</v>
+        <v>456</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -7463,371 +7446,371 @@
         <v>54</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G7" t="s">
         <v>54</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B8" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G8" t="s">
         <v>54</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B9" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G9" t="s">
         <v>54</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B10" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C10" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G10" t="s">
         <v>54</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B11" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G11" t="s">
         <v>54</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B12" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C12" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D12" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G12" t="s">
         <v>54</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B13" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C13" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G13" t="s">
         <v>54</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B14" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C14" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G14" t="s">
         <v>54</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>303</v>
+      </c>
+      <c r="B15" t="s">
+        <v>314</v>
+      </c>
+      <c r="C15" t="s">
+        <v>258</v>
+      </c>
+      <c r="D15" t="s">
         <v>305</v>
-      </c>
-      <c r="B15" t="s">
-        <v>316</v>
-      </c>
-      <c r="C15" t="s">
-        <v>260</v>
-      </c>
-      <c r="D15" t="s">
-        <v>307</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G15" t="s">
         <v>54</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B16" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C16" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D16" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G16" t="s">
         <v>54</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B17" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C17" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D17" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G17" t="s">
         <v>54</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B18" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C18" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D18" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G18" t="s">
         <v>54</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B19" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C19" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D19" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G19" t="s">
         <v>54</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B20" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C20" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D20" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G20" t="s">
         <v>54</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -7848,8 +7831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD424674-210E-914F-938A-C8B62B8D7C97}">
   <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7871,55 +7854,55 @@
         <v>198</v>
       </c>
       <c r="H1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N1" t="s">
         <v>53</v>
       </c>
       <c r="O1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="P1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="Q1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="S1" t="s">
+        <v>229</v>
+      </c>
+      <c r="T1" t="s">
         <v>230</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>231</v>
-      </c>
-      <c r="U1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D2" s="4" t="str">
-        <f>"C"&amp;S2&amp;"H"&amp;T2&amp;"O"&amp;U2</f>
+        <f t="shared" ref="D2:D13" si="0">"C"&amp;S2&amp;"H"&amp;T2&amp;"O"&amp;U2</f>
         <v>C15H26O13</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="O2">
         <v>2</v>
@@ -7928,7 +7911,7 @@
         <v>1</v>
       </c>
       <c r="Q2">
-        <f t="shared" ref="Q2:Q13" si="0">SUM(O2:P2)-1</f>
+        <f t="shared" ref="Q2:Q13" si="1">SUM(O2:P2)-1</f>
         <v>2</v>
       </c>
       <c r="S2">
@@ -7946,23 +7929,23 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D3" s="4" t="str">
-        <f>"C"&amp;S3&amp;"H"&amp;T3&amp;"O"&amp;U3</f>
+        <f t="shared" si="0"/>
         <v>C15H26O13</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J3">
         <v>5</v>
@@ -7971,7 +7954,7 @@
         <v>5</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="O3">
         <v>2</v>
@@ -7980,7 +7963,7 @@
         <v>1</v>
       </c>
       <c r="Q3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="S3">
@@ -7988,33 +7971,33 @@
         <v>15</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:T9" si="1">O3*$J$4+P3*$K$4-2*Q3</f>
+        <f t="shared" ref="T3:T9" si="2">O3*$J$4+P3*$K$4-2*Q3</f>
         <v>26</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U9" si="2">O3*$J$5+P3*$K$5-Q3</f>
+        <f t="shared" ref="U3:U9" si="3">O3*$J$5+P3*$K$5-Q3</f>
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D4" s="4" t="str">
-        <f>"C"&amp;S4&amp;"H"&amp;T4&amp;"O"&amp;U4</f>
+        <f t="shared" si="0"/>
         <v>C20H34O17</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J4">
         <v>10</v>
@@ -8023,7 +8006,7 @@
         <v>10</v>
       </c>
       <c r="N4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="O4">
         <v>3</v>
@@ -8032,41 +8015,41 @@
         <v>1</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="S4">
-        <f t="shared" ref="S4:S9" si="3">O4*$J$3+P4*$K$3</f>
+        <f t="shared" ref="S4:S9" si="4">O4*$J$3+P4*$K$3</f>
         <v>20</v>
       </c>
       <c r="T4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="U4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D5" s="4" t="str">
-        <f>"C"&amp;S5&amp;"H"&amp;T5&amp;"O"&amp;U5</f>
+        <f t="shared" si="0"/>
         <v>C20H34O17</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J5">
         <v>5</v>
@@ -8075,7 +8058,7 @@
         <v>5</v>
       </c>
       <c r="N5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="O5">
         <v>3</v>
@@ -8084,41 +8067,41 @@
         <v>1</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="S5">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="U5">
         <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="T5">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="U5">
-        <f t="shared" si="2"/>
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D6" s="4" t="str">
-        <f>"C"&amp;S6&amp;"H"&amp;T6&amp;"O"&amp;U6</f>
+        <f t="shared" si="0"/>
         <v>C30H50O25</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="N6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="O6">
         <v>4</v>
@@ -8127,41 +8110,41 @@
         <v>2</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="S6">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="U6">
         <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="T6">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="U6">
-        <f t="shared" si="2"/>
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D7" s="4" t="str">
-        <f>"C"&amp;S7&amp;"H"&amp;T7&amp;"O"&amp;U7</f>
+        <f t="shared" si="0"/>
         <v>C30H50O25</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="O7">
         <v>4</v>
@@ -8170,41 +8153,41 @@
         <v>2</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="S7">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="U7">
         <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="T7">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="U7">
-        <f t="shared" si="2"/>
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D8" s="4" t="str">
-        <f>"C"&amp;S8&amp;"H"&amp;T8&amp;"O"&amp;U8</f>
+        <f t="shared" si="0"/>
         <v>C25H42O21</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="O8">
         <v>3</v>
@@ -8213,41 +8196,41 @@
         <v>2</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="S8">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="U8">
         <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-      <c r="T8">
-        <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
-      <c r="U8">
-        <f t="shared" si="2"/>
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D9" s="4" t="str">
-        <f>"C"&amp;S9&amp;"H"&amp;T9&amp;"O"&amp;U9</f>
+        <f t="shared" si="0"/>
         <v>C25H42O21</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="O9" s="4">
         <v>3</v>
@@ -8256,35 +8239,35 @@
         <v>2</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="R9" s="4"/>
       <c r="S9">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="U9">
         <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-      <c r="T9">
-        <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
-      <c r="U9">
-        <f t="shared" si="2"/>
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B10" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D10" s="4" t="str">
-        <f>"C"&amp;S10&amp;"H"&amp;T10&amp;"O"&amp;U10</f>
+        <f t="shared" si="0"/>
         <v>C25H42O21</v>
       </c>
       <c r="E10">
@@ -8296,7 +8279,7 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="N10" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="O10" s="4">
         <v>3</v>
@@ -8305,41 +8288,41 @@
         <v>2</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="S10">
-        <f t="shared" ref="S10" si="4">O10*$J$3+P10*$K$3</f>
+        <f t="shared" ref="S10" si="5">O10*$J$3+P10*$K$3</f>
         <v>25</v>
       </c>
       <c r="T10">
-        <f t="shared" ref="T10" si="5">O10*$J$4+P10*$K$4-2*Q10</f>
+        <f t="shared" ref="T10" si="6">O10*$J$4+P10*$K$4-2*Q10</f>
         <v>42</v>
       </c>
       <c r="U10">
-        <f t="shared" ref="U10" si="6">O10*$J$5+P10*$K$5-Q10</f>
+        <f t="shared" ref="U10" si="7">O10*$J$5+P10*$K$5-Q10</f>
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B11" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D11" s="4" t="str">
-        <f>"C"&amp;S11&amp;"H"&amp;T11&amp;"O"&amp;U11</f>
+        <f t="shared" si="0"/>
         <v>C25H42O21</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="O11">
         <v>4</v>
@@ -8348,7 +8331,7 @@
         <v>1</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="S11">
@@ -8366,16 +8349,16 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B12" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D12" s="4" t="str">
-        <f>"C"&amp;S12&amp;"H"&amp;T12&amp;"O"&amp;U12</f>
+        <f t="shared" si="0"/>
         <v>C25H42O21</v>
       </c>
       <c r="E12">
@@ -8386,7 +8369,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="N12" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O12">
         <v>4</v>
@@ -8395,7 +8378,7 @@
         <v>1</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="S12">
@@ -8413,16 +8396,16 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B13" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D13" s="4" t="str">
-        <f>"C"&amp;S13&amp;"H"&amp;T13&amp;"O"&amp;U13</f>
+        <f t="shared" si="0"/>
         <v>C20H34O17</v>
       </c>
       <c r="E13">
@@ -8430,7 +8413,7 @@
       </c>
       <c r="M13" s="2"/>
       <c r="N13" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="O13">
         <v>3</v>
@@ -8439,7 +8422,7 @@
         <v>1</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="S13">

</xml_diff>